<commit_message>
feat : add INSERT writer and add to init.sql
</commit_message>
<xml_diff>
--- a/datas_to_english/stadium_information.xlsx
+++ b/datas_to_english/stadium_information.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>클럽</t>
   </si>
@@ -22,6 +22,9 @@
     <t>경기장</t>
   </si>
   <si>
+    <t>teamid</t>
+  </si>
+  <si>
     <t>Ulsan</t>
   </si>
   <si>
@@ -158,6 +161,75 @@
   </si>
   <si>
     <t>Gwangyang Stadium</t>
+  </si>
+  <si>
+    <t>7c925ac6-1512-497a-8807-19aee53531d2</t>
+  </si>
+  <si>
+    <t>c67f321d-fab0-4e2a-bdaf-5801469d37b5</t>
+  </si>
+  <si>
+    <t>5b8d0d04-7fc0-4b95-ba05-d124fa4334ac</t>
+  </si>
+  <si>
+    <t>d88ef14f-d2dc-4721-aacc-1f632f7347eb</t>
+  </si>
+  <si>
+    <t>1c104287-7c20-42e4-9fbb-5a9141b323ea</t>
+  </si>
+  <si>
+    <t>7508a993-6eee-47d8-a537-5d5aec6bb902</t>
+  </si>
+  <si>
+    <t>eaa39d6b-eb3b-4ee5-bab1-1908c7aabb73</t>
+  </si>
+  <si>
+    <t>2af463cf-4130-4f2e-9df8-d91f58f98780</t>
+  </si>
+  <si>
+    <t>05d44392-c3eb-4e0e-a3df-28a547d2b0d3</t>
+  </si>
+  <si>
+    <t>7c45e8da-a16c-4a6e-afb9-992af41f1f2b</t>
+  </si>
+  <si>
+    <t>2ba5bbb5-70f8-46c3-b473-907be766d907</t>
+  </si>
+  <si>
+    <t>037f0493-37c7-49c2-a571-bb9a1c67c0e9</t>
+  </si>
+  <si>
+    <t>fe67fd6b-7f29-448c-a4ef-241e6f3e6b43</t>
+  </si>
+  <si>
+    <t>97764f5d-102d-44f7-b018-515714df51bf</t>
+  </si>
+  <si>
+    <t>8130a434-1d36-4aae-b6ad-1aa871f06165</t>
+  </si>
+  <si>
+    <t>b00db273-1041-43c3-b471-4e86d8982b93</t>
+  </si>
+  <si>
+    <t>b9af5cac-c771-40c1-8e03-8c46bd84538d</t>
+  </si>
+  <si>
+    <t>1da80034-143c-4b79-b58a-96a68a75c340</t>
+  </si>
+  <si>
+    <t>b623377a-c762-48a0-9124-9bb8a345dae6</t>
+  </si>
+  <si>
+    <t>8107f4a7-7bb6-4207-940c-f34d2e82a8f0</t>
+  </si>
+  <si>
+    <t>c9986db9-5430-4be4-8bbd-d816e112ac1c</t>
+  </si>
+  <si>
+    <t>82f70bed-ebcd-4751-8245-7221838bc31d</t>
+  </si>
+  <si>
+    <t>f1657738-70c3-46c1-abc4-b8a6a6832705</t>
   </si>
 </sst>
 </file>
@@ -515,271 +587,343 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>45</v>
+      </c>
+      <c r="D21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>46</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>47</v>
+      </c>
+      <c r="D23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="D24" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>